<commit_message>
vault backup: 2023-11-14 10:01:38
</commit_message>
<xml_diff>
--- a/Second year of study/Лабы по Прикладной статистике/лаб 1/лаб1.xlsx
+++ b/Second year of study/Лабы по Прикладной статистике/лаб 1/лаб1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12495"/>
+    <workbookView windowWidth="28125" windowHeight="12495"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="43">
   <si>
     <t>Модель</t>
   </si>
@@ -34,46 +34,115 @@
     <t>Алгоритм хеширования</t>
   </si>
   <si>
-    <t>Bitmain Antminer L7 9050</t>
+    <t>Antminer L7 9050</t>
   </si>
   <si>
     <t>Scrypt</t>
   </si>
   <si>
-    <t>Bitmain Antminer E9 Pro</t>
+    <t>Antminer E9 Pro</t>
   </si>
   <si>
     <t>Ethash</t>
   </si>
   <si>
-    <t xml:space="preserve">Bitmain Antminer E9 </t>
-  </si>
-  <si>
-    <t>Bitmain Antminer E9</t>
+    <t xml:space="preserve">Antminer E9 </t>
+  </si>
+  <si>
+    <t>Antminer E9</t>
   </si>
   <si>
     <t>SHA-256</t>
   </si>
   <si>
-    <t>Bitmain Antminer S19k Pro</t>
-  </si>
-  <si>
-    <t>Bitmain Antminer Z15 Pro</t>
+    <t>Antminer S19k Pro</t>
+  </si>
+  <si>
+    <t>Antminer Z15 Pro</t>
   </si>
   <si>
     <t>Equilhash</t>
   </si>
   <si>
-    <t>Bitmain Antminer Z15</t>
-  </si>
-  <si>
-    <t>MicroBT Whatsminer M50</t>
-  </si>
-  <si>
-    <t>Bitmain Antminer S19j Pro</t>
-  </si>
-  <si>
-    <t>MicroBT Whatsminer M30S++ 112</t>
+    <t>Antminer Z15</t>
+  </si>
+  <si>
+    <t>Whatsminer M50</t>
+  </si>
+  <si>
+    <t>Antminer S19j Pro</t>
+  </si>
+  <si>
+    <t>Whatsminer M30S++ 112</t>
+  </si>
+  <si>
+    <t>Antminer KS3</t>
+  </si>
+  <si>
+    <t>KHeavyHash</t>
+  </si>
+  <si>
+    <t>iPollo v1</t>
+  </si>
+  <si>
+    <t>Antminer S19 XP Hyd</t>
+  </si>
+  <si>
+    <t>Antiminer L7</t>
+  </si>
+  <si>
+    <t>Whatsminer 56S</t>
+  </si>
+  <si>
+    <t>Whatsminer 53S</t>
+  </si>
+  <si>
+    <t>Antminer D9</t>
+  </si>
+  <si>
+    <t>X11</t>
+  </si>
+  <si>
+    <t>Antminer E7</t>
+  </si>
+  <si>
+    <t>Antminer D7</t>
+  </si>
+  <si>
+    <t>Antminer KA3</t>
+  </si>
+  <si>
+    <t>Bake2s</t>
+  </si>
+  <si>
+    <t>Whatsminer M50S</t>
+  </si>
+  <si>
+    <t>iPollo G1</t>
+  </si>
+  <si>
+    <t>Cuckatoo32</t>
+  </si>
+  <si>
+    <t>Whatsminer M31S</t>
+  </si>
+  <si>
+    <t>Innosilicon A11 Pro</t>
+  </si>
+  <si>
+    <t>Whatsminer M20S</t>
+  </si>
+  <si>
+    <t>Hammer D10+</t>
+  </si>
+  <si>
+    <t>Jasminer X4</t>
+  </si>
+  <si>
+    <t>Avalon Made A1366I</t>
+  </si>
+  <si>
+    <t>Innosilicon A10 Pro</t>
   </si>
 </sst>
 </file>
@@ -81,14 +150,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="0.0"/>
-    <numFmt numFmtId="177" formatCode="_-* #\.##0.00\ &quot;₽&quot;_-;\-* #\.##0.00\ &quot;₽&quot;_-;_-* \-??\ &quot;₽&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #\.##0_-;\-* #\.##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-* #\.##0\ &quot;₽&quot;_-;\-* #\.##0\ &quot;₽&quot;_-;_-* \-\ &quot;₽&quot;_-;_-@_-"/>
-    <numFmt numFmtId="180" formatCode="_-* #\.##0.00_-;\-* #\.##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="181" formatCode="0.0%"/>
+    <numFmt numFmtId="176" formatCode="_-* #\.##0.00\ &quot;₽&quot;_-;\-* #\.##0.00\ &quot;₽&quot;_-;_-* \-??\ &quot;₽&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #\.##0\ &quot;₽&quot;_-;\-* #\.##0\ &quot;₽&quot;_-;_-* \-\ &quot;₽&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #\.##0.00_-;\-* #\.##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="0.0%"/>
+    <numFmt numFmtId="180" formatCode="_-* #\.##0_-;\-* #\.##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="181" formatCode="0.0"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,8 +172,50 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF272323"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -118,20 +229,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,6 +237,37 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -149,53 +277,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -234,18 +316,11 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -256,55 +331,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -316,127 +511,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -466,6 +541,30 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -476,21 +575,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -507,16 +591,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -553,66 +637,57 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -621,98 +696,98 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -722,10 +797,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="181" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
@@ -737,10 +812,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="181" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="181" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -809,7 +893,7 @@
         <sz val="12"/>
         <color theme="1"/>
       </font>
-      <numFmt numFmtId="176" formatCode="0.0"/>
+      <numFmt numFmtId="181" formatCode="0.0"/>
       <border>
         <left style="thin">
           <color auto="1"/>
@@ -838,7 +922,7 @@
         <sz val="12"/>
         <color theme="1"/>
       </font>
-      <numFmt numFmtId="176" formatCode="0.0"/>
+      <numFmt numFmtId="181" formatCode="0.0"/>
       <border>
         <left style="thin">
           <color auto="1"/>
@@ -896,7 +980,7 @@
         <sz val="12"/>
         <color theme="1"/>
       </font>
-      <numFmt numFmtId="176" formatCode="0.0"/>
+      <numFmt numFmtId="181" formatCode="0.0"/>
       <border>
         <left style="thin">
           <color auto="1"/>
@@ -925,7 +1009,7 @@
         <sz val="12"/>
         <color theme="1"/>
       </font>
-      <numFmt numFmtId="176" formatCode="0.0"/>
+      <numFmt numFmtId="181" formatCode="0.0"/>
       <border>
         <left style="thin">
           <color auto="1"/>
@@ -952,8 +1036,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="УТ_Данные" displayName="УТ_Данные" ref="A1:F11" totalsRowShown="0">
-  <autoFilter ref="A1:F11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="УТ_Данные" displayName="УТ_Данные" ref="A1:F30" totalsRowShown="0">
+  <autoFilter ref="A1:F30"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Модель"/>
     <tableColumn id="2" name="Хешрейт, Mh/s" dataDxfId="0"/>
@@ -1227,7 +1311,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15.75" outlineLevelCol="5"/>
@@ -1272,7 +1356,7 @@
         <v>3300</v>
       </c>
       <c r="D2" s="5">
-        <v>0.36</v>
+        <v>35</v>
       </c>
       <c r="E2" s="4">
         <v>424373</v>
@@ -1292,7 +1376,7 @@
         <v>2200</v>
       </c>
       <c r="D3" s="5">
-        <v>0.6</v>
+        <v>60</v>
       </c>
       <c r="E3" s="4">
         <v>206855</v>
@@ -1312,7 +1396,7 @@
         <v>1920</v>
       </c>
       <c r="D4" s="5">
-        <v>0.85</v>
+        <v>85</v>
       </c>
       <c r="E4" s="4">
         <v>96671</v>
@@ -1372,7 +1456,7 @@
         <v>2650</v>
       </c>
       <c r="D7" s="5">
-        <v>3.15</v>
+        <v>31.5</v>
       </c>
       <c r="E7" s="4">
         <v>252008</v>
@@ -1392,7 +1476,7 @@
         <v>2650</v>
       </c>
       <c r="D8" s="5">
-        <v>3.72</v>
+        <v>37.2</v>
       </c>
       <c r="E8" s="4">
         <v>243411</v>
@@ -1441,7 +1525,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" ht="31.5" spans="1:6">
+    <row r="11" spans="1:6">
       <c r="A11" s="6" t="s">
         <v>19</v>
       </c>
@@ -1461,152 +1545,399 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="7"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="7"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="7"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="7"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="7"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="7"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="7"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="7"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="7"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="7"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="7"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="7"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="7"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="7"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="7"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="7"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
+    <row r="12" spans="1:6">
+      <c r="A12" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="4">
+        <v>83000</v>
+      </c>
+      <c r="C12" s="4">
+        <v>3188</v>
+      </c>
+      <c r="D12" s="5">
+        <v>38</v>
+      </c>
+      <c r="E12" s="4">
+        <v>3500000</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="4">
+        <v>3600</v>
+      </c>
+      <c r="C13" s="4">
+        <v>2400</v>
+      </c>
+      <c r="D13" s="5">
+        <v>86.1</v>
+      </c>
+      <c r="E13" s="4">
+        <v>672603</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="4">
+        <v>25700</v>
+      </c>
+      <c r="C14" s="4">
+        <v>5300</v>
+      </c>
+      <c r="D14" s="5">
+        <v>20.8</v>
+      </c>
+      <c r="E14" s="4">
+        <v>486948</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="4">
+        <v>9050</v>
+      </c>
+      <c r="C15" s="4">
+        <v>3300</v>
+      </c>
+      <c r="D15" s="5">
+        <v>36</v>
+      </c>
+      <c r="E15" s="4">
+        <v>408879</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="4">
+        <v>20000</v>
+      </c>
+      <c r="C16" s="4">
+        <v>5550</v>
+      </c>
+      <c r="D16" s="5">
+        <v>26</v>
+      </c>
+      <c r="E16" s="4">
+        <v>403922</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="4">
+        <v>25000</v>
+      </c>
+      <c r="C17" s="4">
+        <v>7250</v>
+      </c>
+      <c r="D17" s="5">
+        <v>29</v>
+      </c>
+      <c r="E17" s="4">
+        <v>350000</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="4">
+        <v>17000</v>
+      </c>
+      <c r="C18" s="4">
+        <v>2839</v>
+      </c>
+      <c r="D18" s="5">
+        <v>17.7</v>
+      </c>
+      <c r="E18" s="4">
+        <v>348246</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="4">
+        <v>800</v>
+      </c>
+      <c r="C19" s="4">
+        <v>1300</v>
+      </c>
+      <c r="D19" s="5">
+        <v>27</v>
+      </c>
+      <c r="E19" s="4">
+        <v>285115</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="4">
+        <v>12680</v>
+      </c>
+      <c r="C20" s="4">
+        <v>31448</v>
+      </c>
+      <c r="D20" s="5">
+        <v>52</v>
+      </c>
+      <c r="E20" s="4">
+        <v>279854</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="4">
+        <v>16600</v>
+      </c>
+      <c r="C21" s="4">
+        <v>3154</v>
+      </c>
+      <c r="D21" s="5">
+        <v>19</v>
+      </c>
+      <c r="E21" s="4">
+        <v>269470</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="4">
+        <v>13000</v>
+      </c>
+      <c r="C22" s="4">
+        <v>3276</v>
+      </c>
+      <c r="D22" s="5">
+        <v>34.3</v>
+      </c>
+      <c r="E22" s="4">
+        <v>198723</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="4">
+        <v>3600</v>
+      </c>
+      <c r="C23" s="4">
+        <v>2800</v>
+      </c>
+      <c r="D23" s="5">
+        <v>41</v>
+      </c>
+      <c r="E23" s="4">
+        <v>1780000</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="4">
+        <v>7000</v>
+      </c>
+      <c r="C24" s="4">
+        <v>3276</v>
+      </c>
+      <c r="D24" s="5">
+        <v>45</v>
+      </c>
+      <c r="E24" s="4">
+        <v>106845</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="4">
+        <v>1500</v>
+      </c>
+      <c r="C25" s="4">
+        <v>2350</v>
+      </c>
+      <c r="D25" s="5">
+        <v>15.6</v>
+      </c>
+      <c r="E25" s="4">
+        <v>100263</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="4">
+        <v>6800</v>
+      </c>
+      <c r="C26" s="4">
+        <v>3200</v>
+      </c>
+      <c r="D26" s="5">
+        <v>48</v>
+      </c>
+      <c r="E26" s="4">
+        <v>52766</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="4">
+        <v>5000</v>
+      </c>
+      <c r="C27" s="4">
+        <v>3700</v>
+      </c>
+      <c r="D27" s="5">
+        <v>74</v>
+      </c>
+      <c r="E27" s="4">
+        <v>276406</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="4">
+        <v>5400</v>
+      </c>
+      <c r="C28" s="4">
+        <v>240</v>
+      </c>
+      <c r="D28" s="5">
+        <v>32.5</v>
+      </c>
+      <c r="E28" s="4">
+        <v>272340</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="4">
+        <v>16500</v>
+      </c>
+      <c r="C29" s="4">
+        <v>4950</v>
+      </c>
+      <c r="D29" s="5">
+        <v>30</v>
+      </c>
+      <c r="E29" s="4">
+        <v>220000</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B30" s="4">
+        <v>500</v>
+      </c>
+      <c r="C30" s="4">
+        <v>950</v>
+      </c>
+      <c r="D30" s="5">
+        <v>65</v>
+      </c>
+      <c r="E30" s="4">
+        <v>122553</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="7"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="7"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
vault backup: 2023-11-14 14:07:44
</commit_message>
<xml_diff>
--- a/Second year of study/Лабы по Прикладной статистике/лаб 1/лаб1.xlsx
+++ b/Second year of study/Лабы по Прикладной статистике/лаб 1/лаб1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12495"/>
+    <workbookView windowWidth="28800" windowHeight="12495"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="44">
   <si>
     <t>Модель</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>Innosilicon A10 Pro</t>
+  </si>
+  <si>
+    <t>Goldshell LT5 Pro</t>
   </si>
 </sst>
 </file>
@@ -151,13 +154,13 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
     <numFmt numFmtId="176" formatCode="_-* #\.##0.00\ &quot;₽&quot;_-;\-* #\.##0.00\ &quot;₽&quot;_-;_-* \-??\ &quot;₽&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #\.##0\ &quot;₽&quot;_-;\-* #\.##0\ &quot;₽&quot;_-;_-* \-\ &quot;₽&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #\.##0.00_-;\-* #\.##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="0.0%"/>
-    <numFmt numFmtId="180" formatCode="_-* #\.##0_-;\-* #\.##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="181" formatCode="0.0"/>
+    <numFmt numFmtId="177" formatCode="_-* #\.##0_-;\-* #\.##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #\.##0\ &quot;₽&quot;_-;\-* #\.##0\ &quot;₽&quot;_-;_-* \-\ &quot;₽&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="0.0"/>
+    <numFmt numFmtId="180" formatCode="_-* #\.##0.00_-;\-* #\.##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="181" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,8 +181,49 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -194,30 +238,80 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -229,98 +323,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -331,61 +339,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -397,121 +513,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -536,30 +544,6 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -591,6 +575,30 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -601,6 +609,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -622,168 +645,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -797,10 +805,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
@@ -812,19 +820,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="181" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -893,7 +901,7 @@
         <sz val="12"/>
         <color theme="1"/>
       </font>
-      <numFmt numFmtId="181" formatCode="0.0"/>
+      <numFmt numFmtId="179" formatCode="0.0"/>
       <border>
         <left style="thin">
           <color auto="1"/>
@@ -922,7 +930,7 @@
         <sz val="12"/>
         <color theme="1"/>
       </font>
-      <numFmt numFmtId="181" formatCode="0.0"/>
+      <numFmt numFmtId="179" formatCode="0.0"/>
       <border>
         <left style="thin">
           <color auto="1"/>
@@ -980,7 +988,7 @@
         <sz val="12"/>
         <color theme="1"/>
       </font>
-      <numFmt numFmtId="181" formatCode="0.0"/>
+      <numFmt numFmtId="179" formatCode="0.0"/>
       <border>
         <left style="thin">
           <color auto="1"/>
@@ -1009,7 +1017,7 @@
         <sz val="12"/>
         <color theme="1"/>
       </font>
-      <numFmt numFmtId="181" formatCode="0.0"/>
+      <numFmt numFmtId="179" formatCode="0.0"/>
       <border>
         <left style="thin">
           <color auto="1"/>
@@ -1036,8 +1044,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="УТ_Данные" displayName="УТ_Данные" ref="A1:F30" totalsRowShown="0">
-  <autoFilter ref="A1:F30"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="УТ_Данные" displayName="УТ_Данные" ref="A1:F31" totalsRowShown="0">
+  <autoFilter ref="A1:F31"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Модель"/>
     <tableColumn id="2" name="Хешрейт, Mh/s" dataDxfId="0"/>
@@ -1311,7 +1319,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15.75" outlineLevelCol="5"/>
@@ -1561,7 +1569,7 @@
       <c r="E12" s="4">
         <v>3500000</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="4" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1581,12 +1589,12 @@
       <c r="E13" s="4">
         <v>672603</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="8" t="s">
         <v>23</v>
       </c>
       <c r="B14" s="4">
@@ -1601,7 +1609,7 @@
       <c r="E14" s="4">
         <v>486948</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="9" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1621,7 +1629,7 @@
       <c r="E15" s="4">
         <v>408879</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1641,7 +1649,7 @@
       <c r="E16" s="4">
         <v>403922</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1661,7 +1669,7 @@
       <c r="E17" s="4">
         <v>350000</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F17" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1681,7 +1689,7 @@
       <c r="E18" s="4">
         <v>348246</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F18" s="4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1701,7 +1709,7 @@
       <c r="E19" s="4">
         <v>285115</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F19" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1721,7 +1729,7 @@
       <c r="E20" s="4">
         <v>279854</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F20" s="4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1741,7 +1749,7 @@
       <c r="E21" s="4">
         <v>269470</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F21" s="4" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1761,7 +1769,7 @@
       <c r="E22" s="4">
         <v>198723</v>
       </c>
-      <c r="F22" s="8" t="s">
+      <c r="F22" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1781,7 +1789,7 @@
       <c r="E23" s="4">
         <v>1780000</v>
       </c>
-      <c r="F23" s="8" t="s">
+      <c r="F23" s="4" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1801,7 +1809,7 @@
       <c r="E24" s="4">
         <v>106845</v>
       </c>
-      <c r="F24" s="8" t="s">
+      <c r="F24" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1821,7 +1829,7 @@
       <c r="E25" s="4">
         <v>100263</v>
       </c>
-      <c r="F25" s="8" t="s">
+      <c r="F25" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1841,7 +1849,7 @@
       <c r="E26" s="4">
         <v>52766</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="F26" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1861,7 +1869,7 @@
       <c r="E27" s="4">
         <v>276406</v>
       </c>
-      <c r="F27" s="8" t="s">
+      <c r="F27" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1881,7 +1889,7 @@
       <c r="E28" s="4">
         <v>272340</v>
       </c>
-      <c r="F28" s="8" t="s">
+      <c r="F28" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1901,7 +1909,7 @@
       <c r="E29" s="4">
         <v>220000</v>
       </c>
-      <c r="F29" s="8" t="s">
+      <c r="F29" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1921,16 +1929,29 @@
       <c r="E30" s="4">
         <v>122553</v>
       </c>
-      <c r="F30" s="8" t="s">
+      <c r="F30" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="7"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
+    <row r="31" spans="1:6">
+      <c r="A31" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="4">
+        <v>24500</v>
+      </c>
+      <c r="C31" s="4">
+        <v>3100</v>
+      </c>
+      <c r="D31" s="5">
+        <v>22.3</v>
+      </c>
+      <c r="E31" s="4">
+        <v>302978</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="7"/>
@@ -1940,6 +1961,9 @@
       <c r="E32" s="12"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A31" r:id="rId2" display="Goldshell LT5 Pro" tooltip="https://ibmm.ru/katalog/goldshell/goldshell-lt-5-pro/"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
   <tableParts count="1">

</xml_diff>

<commit_message>
vault backup: 2023-11-14 16:55:55
</commit_message>
<xml_diff>
--- a/Second year of study/Лабы по Прикладной статистике/лаб 1/лаб1.xlsx
+++ b/Second year of study/Лабы по Прикладной статистике/лаб 1/лаб1.xlsx
@@ -7,7 +7,7 @@
     <workbookView windowWidth="28800" windowHeight="12495"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Данные" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -153,12 +153,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="_-* #\.##0.00\ &quot;₽&quot;_-;\-* #\.##0.00\ &quot;₽&quot;_-;_-* \-??\ &quot;₽&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #\.##0_-;\-* #\.##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #\.##0\ &quot;₽&quot;_-;\-* #\.##0\ &quot;₽&quot;_-;_-* \-\ &quot;₽&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="0.0"/>
-    <numFmt numFmtId="180" formatCode="_-* #\.##0.00_-;\-* #\.##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="181" formatCode="0.0%"/>
+    <numFmt numFmtId="176" formatCode="0.0"/>
+    <numFmt numFmtId="177" formatCode="_-* #\.##0.00_-;\-* #\.##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #\.##0.00\ &quot;₽&quot;_-;\-* #\.##0.00\ &quot;₽&quot;_-;_-* \-??\ &quot;₽&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="0.0%"/>
+    <numFmt numFmtId="180" formatCode="_-* #\.##0_-;\-* #\.##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="181" formatCode="_-* #\.##0\ &quot;₽&quot;_-;\-* #\.##0\ &quot;₽&quot;_-;_-* \-\ &quot;₽&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -187,28 +187,37 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -229,21 +238,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -260,6 +254,45 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -268,53 +301,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -324,6 +310,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -339,12 +339,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -357,163 +375,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -544,6 +544,30 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -575,30 +599,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -609,6 +609,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -631,17 +640,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -650,152 +650,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -805,10 +805,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
@@ -829,10 +829,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -901,7 +898,7 @@
         <sz val="12"/>
         <color theme="1"/>
       </font>
-      <numFmt numFmtId="179" formatCode="0.0"/>
+      <numFmt numFmtId="176" formatCode="0.0"/>
       <border>
         <left style="thin">
           <color auto="1"/>
@@ -930,7 +927,7 @@
         <sz val="12"/>
         <color theme="1"/>
       </font>
-      <numFmt numFmtId="179" formatCode="0.0"/>
+      <numFmt numFmtId="176" formatCode="0.0"/>
       <border>
         <left style="thin">
           <color auto="1"/>
@@ -988,7 +985,7 @@
         <sz val="12"/>
         <color theme="1"/>
       </font>
-      <numFmt numFmtId="179" formatCode="0.0"/>
+      <numFmt numFmtId="176" formatCode="0.0"/>
       <border>
         <left style="thin">
           <color auto="1"/>
@@ -1017,7 +1014,7 @@
         <sz val="12"/>
         <color theme="1"/>
       </font>
-      <numFmt numFmtId="179" formatCode="0.0"/>
+      <numFmt numFmtId="176" formatCode="0.0"/>
       <border>
         <left style="thin">
           <color auto="1"/>
@@ -1319,7 +1316,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15.75" outlineLevelCol="5"/>
@@ -1418,7 +1415,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="4">
-        <v>140000</v>
+        <v>14000</v>
       </c>
       <c r="C5" s="4">
         <v>3010</v>
@@ -1438,7 +1435,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="4">
-        <v>136000</v>
+        <v>13600</v>
       </c>
       <c r="C6" s="4">
         <v>3264</v>
@@ -1458,7 +1455,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="4">
-        <v>840000</v>
+        <v>84000</v>
       </c>
       <c r="C7" s="4">
         <v>2650</v>
@@ -1478,7 +1475,7 @@
         <v>16</v>
       </c>
       <c r="B8" s="4">
-        <v>420000</v>
+        <v>42000</v>
       </c>
       <c r="C8" s="4">
         <v>2650</v>
@@ -1498,7 +1495,7 @@
         <v>17</v>
       </c>
       <c r="B9" s="4">
-        <v>118000</v>
+        <v>11800</v>
       </c>
       <c r="C9" s="4">
         <v>3306</v>
@@ -1518,7 +1515,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="4">
-        <v>104000</v>
+        <v>10400</v>
       </c>
       <c r="C10" s="4">
         <v>3250</v>
@@ -1538,7 +1535,7 @@
         <v>19</v>
       </c>
       <c r="B11" s="4">
-        <v>112000</v>
+        <v>11200</v>
       </c>
       <c r="C11" s="4">
         <v>3472</v>
@@ -1949,16 +1946,16 @@
       <c r="E31" s="4">
         <v>302978</v>
       </c>
-      <c r="F31" s="11" t="s">
+      <c r="F31" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="7"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
vault backup: 2023-11-28 16:48:45
</commit_message>
<xml_diff>
--- a/Second year of study/Лабы по Прикладной статистике/лаб 1/лаб1.xlsx
+++ b/Second year of study/Лабы по Прикладной статистике/лаб 1/лаб1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12495"/>
+    <workbookView windowWidth="23820" windowHeight="12495"/>
   </bookViews>
   <sheets>
     <sheet name="Данные" sheetId="1" r:id="rId1"/>
@@ -154,11 +154,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
     <numFmt numFmtId="176" formatCode="0.0"/>
-    <numFmt numFmtId="177" formatCode="_-* #\.##0.00_-;\-* #\.##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #\.##0.00\ &quot;₽&quot;_-;\-* #\.##0.00\ &quot;₽&quot;_-;_-* \-??\ &quot;₽&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="0.0%"/>
-    <numFmt numFmtId="180" formatCode="_-* #\.##0_-;\-* #\.##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="181" formatCode="_-* #\.##0\ &quot;₽&quot;_-;\-* #\.##0\ &quot;₽&quot;_-;_-* \-\ &quot;₽&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #\.##0.00\ &quot;₽&quot;_-;\-* #\.##0.00\ &quot;₽&quot;_-;_-* \-??\ &quot;₽&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="0.0%"/>
+    <numFmt numFmtId="179" formatCode="_-* #\.##0_-;\-* #\.##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="180" formatCode="_-* #\.##0\ &quot;₽&quot;_-;\-* #\.##0\ &quot;₽&quot;_-;_-* \-\ &quot;₽&quot;_-;_-@_-"/>
+    <numFmt numFmtId="181" formatCode="_-* #\.##0.00_-;\-* #\.##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -187,14 +187,45 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -208,6 +239,37 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -216,67 +278,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -293,6 +294,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -301,7 +309,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -310,13 +317,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -339,19 +339,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -363,19 +411,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -387,24 +423,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -417,6 +435,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -435,18 +459,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -465,7 +477,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -501,19 +513,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -544,30 +544,6 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -599,6 +575,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -609,6 +600,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -650,67 +650,67 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="181" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -719,79 +719,79 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -829,7 +829,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1316,7 +1316,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15.75" outlineLevelCol="5"/>
@@ -1878,7 +1878,7 @@
         <v>5400</v>
       </c>
       <c r="C28" s="4">
-        <v>240</v>
+        <v>2400</v>
       </c>
       <c r="D28" s="5">
         <v>32.5</v>

</xml_diff>